<commit_message>
Upload before pulling files from BC Cert DB Server
</commit_message>
<xml_diff>
--- a/Data Extraction And Loading/Program Files/Documentation/Data Loading CheckList (Incremental).xlsx
+++ b/Data Extraction And Loading/Program Files/Documentation/Data Loading CheckList (Incremental).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck\Documents\ROC\Speedway-Source\Data Extraction And Loading\Program Files\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4BA8A8-C448-479B-8DF2-6DC0618E7FC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141782A8-5519-4C0F-9BF7-F1A9E90BE861}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="864" yWindow="360" windowWidth="21600" windowHeight="11652" xr2:uid="{35CC5D13-6FA0-4E86-8B8E-1E92ADCCBFD3}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="23010" windowHeight="12360" xr2:uid="{35CC5D13-6FA0-4E86-8B8E-1E92ADCCBFD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete Load" sheetId="1" r:id="rId1"/>
@@ -774,23 +774,23 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F24:F26"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="31.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="31.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="47.77734375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="29.109375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="38.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="47.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -813,7 +813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -836,7 +836,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -853,7 +853,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -876,7 +876,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -899,7 +899,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -919,7 +919,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -939,7 +939,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -962,7 +962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -985,7 +985,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1456,31 +1456,31 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
     </row>
   </sheetData>

</xml_diff>